<commit_message>
[Undone] Re-organize source code
</commit_message>
<xml_diff>
--- a/source/PythonDataQualityChecker.xlsx
+++ b/source/PythonDataQualityChecker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -743,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -818,7 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>